<commit_message>
Teammeeting protokoll und Zeitblatt
</commit_message>
<xml_diff>
--- a/Zeitblaetter/Ursus Schneider.xlsx
+++ b/Zeitblaetter/Ursus Schneider.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1620" yWindow="940" windowWidth="29640" windowHeight="17940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Datum</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>14:00 - 15:30</t>
+  </si>
+  <si>
+    <t>UART problem nachgehen</t>
+  </si>
+  <si>
+    <t>17:00 - 19:00</t>
+  </si>
+  <si>
+    <t>14:00 - 16:30</t>
+  </si>
+  <si>
+    <t>Teammeating, zusammenführen UART und RF</t>
   </si>
 </sst>
 </file>
@@ -970,7 +982,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,32 +1271,59 @@
         <f t="shared" si="0"/>
         <v>42702</v>
       </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42703</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>42704</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>2.5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="2">
         <f>SUM(B4:B34)</f>
-        <v>26.75</v>
+        <v>32.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>